<commit_message>
update the format for windows
</commit_message>
<xml_diff>
--- a/C-201 airflow analysis.xlsx
+++ b/C-201 airflow analysis.xlsx
@@ -2238,7 +2238,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L38" sqref="L38"/>
+      <selection pane="bottomLeft" activeCell="AJ28" sqref="AJ28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -4071,6 +4071,10 @@
         <f t="shared" si="6"/>
         <v>0.34385060405218726</v>
       </c>
+      <c r="AJ27" s="1">
+        <f>-28.8*98.06</f>
+        <v>-2824.1280000000002</v>
+      </c>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A28" s="14">
@@ -4188,6 +4192,10 @@
       <c r="AI28" s="103">
         <f t="shared" si="6"/>
         <v>0.35680588829191545</v>
+      </c>
+      <c r="AJ28" s="1">
+        <f>101000+AJ27</f>
+        <v>98175.872000000003</v>
       </c>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.2">

</xml_diff>